<commit_message>
Added arch/avr/px_gpio_init_atmega328p.h to calculate GPIO register initialization values
</commit_message>
<xml_diff>
--- a/boards/avr/arduino_uno_board/px_board_gpio.xlsx
+++ b/boards/avr/arduino_uno_board/px_board_gpio.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67AD4B2C-711F-450D-B0C6-439F6756C230}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GPIO" sheetId="7" r:id="rId1"/>
@@ -14,12 +15,20 @@
     <definedName name="Dir">Options!$A$2:$A$3</definedName>
     <definedName name="Init">Options!$C$2:$C$5</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -30,9 +39,6 @@
     <t>Pin</t>
   </si>
   <si>
-    <t>Code</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
@@ -127,12 +133,21 @@
   </si>
   <si>
     <t>PX_GPIO_D7</t>
+  </si>
+  <si>
+    <t>Definitions</t>
+  </si>
+  <si>
+    <t>Global variables</t>
+  </si>
+  <si>
+    <t>Map</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -358,6 +373,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -393,6 +425,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -568,11 +617,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC0A020"/>
   </sheetPr>
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
@@ -589,10 +638,14 @@
     <col min="7" max="7" width="2.7109375" style="3" customWidth="1"/>
     <col min="8" max="8" width="3.85546875" style="3" customWidth="1"/>
     <col min="9" max="9" width="59.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="3"/>
+    <col min="10" max="10" width="9.140625" style="3"/>
+    <col min="11" max="11" width="54.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="3"/>
+    <col min="13" max="13" width="31.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -603,37 +656,43 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="2"/>
       <c r="I1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>4</v>
       </c>
       <c r="C2" s="4">
         <v>0</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" s="6">
         <f>VLOOKUP(D2,Options!A$2:B$100,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" s="6">
         <f>VLOOKUP(F2,Options!C$2:D$100,2,FALSE)</f>
@@ -644,26 +703,34 @@
         <f t="shared" ref="I2:I7" si="0">CONCATENATE("#define ",A2," GPIO(",B2,", ",C2,", ",D2,", ",F2,")")</f>
         <v>#define PX_GPIO_D8 GPIO(B, 0, PX_GPIO_DIR_IN, PX_GPIO_INIT_PULLUP)</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K2" s="3" t="str">
+        <f>CONCATENATE("static const px_gpio_handle_t ",LOWER($A2)," = {",$A2,"};")</f>
+        <v>static const px_gpio_handle_t px_gpio_d8 = {PX_GPIO_D8};</v>
+      </c>
+      <c r="M2" s="3" t="str">
+        <f>CONCATENATE("#define PX_GPIO_",$B2,$C2," ",$A2)</f>
+        <v>#define PX_GPIO_B0 PX_GPIO_D8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="4">
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="6">
         <f>VLOOKUP(D3,Options!A$2:B$100,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" s="6">
         <f>VLOOKUP(F3,Options!C$2:D$100,2,FALSE)</f>
@@ -674,26 +741,34 @@
         <f t="shared" si="0"/>
         <v>#define PX_GPIO_D9 GPIO(B, 1, PX_GPIO_DIR_IN, PX_GPIO_INIT_PULLUP)</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K3" s="3" t="str">
+        <f t="shared" ref="K3:K15" si="1">CONCATENATE("static const px_gpio_handle_t ",LOWER($A3)," = {",$A3,"};")</f>
+        <v>static const px_gpio_handle_t px_gpio_d9 = {PX_GPIO_D9};</v>
+      </c>
+      <c r="M3" s="3" t="str">
+        <f t="shared" ref="M3:M15" si="2">CONCATENATE("#define PX_GPIO_",$B3,$C3," ",$A3)</f>
+        <v>#define PX_GPIO_B1 PX_GPIO_D9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="4">
         <v>2</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="6">
         <f>VLOOKUP(D4,Options!A$2:B$100,2,FALSE)</f>
         <v>2</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4" s="6">
         <f>VLOOKUP(F4,Options!C$2:D$100,2,FALSE)</f>
@@ -704,26 +779,34 @@
         <f t="shared" si="0"/>
         <v>#define PX_GPIO_SPI_SS GPIO(B, 2, PX_GPIO_DIR_OUT, PX_GPIO_INIT_HI)</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K4" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>static const px_gpio_handle_t px_gpio_spi_ss = {PX_GPIO_SPI_SS};</v>
+      </c>
+      <c r="M4" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_B2 PX_GPIO_SPI_SS</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="4">
         <v>3</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" s="6">
         <f>VLOOKUP(D5,Options!A$2:B$100,2,FALSE)</f>
         <v>2</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" s="6">
         <f>VLOOKUP(F5,Options!C$2:D$100,2,FALSE)</f>
@@ -734,26 +817,34 @@
         <f t="shared" si="0"/>
         <v>#define PX_GPIO_SPIO_MOSI GPIO(B, 3, PX_GPIO_DIR_OUT, PX_GPIO_INIT_LO)</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K5" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>static const px_gpio_handle_t px_gpio_spio_mosi = {PX_GPIO_SPIO_MOSI};</v>
+      </c>
+      <c r="M5" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_B3 PX_GPIO_SPIO_MOSI</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="4">
         <v>4</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" s="6">
         <f>VLOOKUP(D6,Options!A$2:B$100,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G6" s="6">
         <f>VLOOKUP(F6,Options!C$2:D$100,2,FALSE)</f>
@@ -764,26 +855,34 @@
         <f t="shared" si="0"/>
         <v>#define PX_GPIO_SPI_MISO GPIO(B, 4, PX_GPIO_DIR_IN, PX_GPIO_INIT_HIZ)</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K6" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>static const px_gpio_handle_t px_gpio_spi_miso = {PX_GPIO_SPI_MISO};</v>
+      </c>
+      <c r="M6" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_B4 PX_GPIO_SPI_MISO</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" s="4">
         <v>5</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" s="6">
         <f>VLOOKUP(D7,Options!A$2:B$100,2,FALSE)</f>
         <v>2</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7" s="6">
         <f>VLOOKUP(F7,Options!C$2:D$100,2,FALSE)</f>
@@ -794,26 +893,34 @@
         <f t="shared" si="0"/>
         <v>#define PX_GPIO_SPI_SCK GPIO(B, 5, PX_GPIO_DIR_OUT, PX_GPIO_INIT_LO)</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K7" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>static const px_gpio_handle_t px_gpio_spi_sck = {PX_GPIO_SPI_SCK};</v>
+      </c>
+      <c r="M7" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_B5 PX_GPIO_SPI_SCK</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" s="4">
         <v>5</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" s="6">
         <f>VLOOKUP(D8,Options!A$2:B$100,2,FALSE)</f>
         <v>2</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G8" s="6">
         <f>VLOOKUP(F8,Options!C$2:D$100,2,FALSE)</f>
@@ -821,29 +928,37 @@
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="3" t="str">
-        <f t="shared" ref="I8" si="1">CONCATENATE("#define ",A8," GPIO(",B8,", ",C8,", ",D8,", ",F8,")")</f>
+        <f t="shared" ref="I8" si="3">CONCATENATE("#define ",A8," GPIO(",B8,", ",C8,", ",D8,", ",F8,")")</f>
         <v>#define PX_GPIO_LED GPIO(B, 5, PX_GPIO_DIR_OUT, PX_GPIO_INIT_LO)</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K8" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>static const px_gpio_handle_t px_gpio_led = {PX_GPIO_LED};</v>
+      </c>
+      <c r="M8" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_B5 PX_GPIO_LED</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="4">
         <v>0</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" s="6">
         <f>VLOOKUP(D10,Options!A$2:B$100,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G10" s="6">
         <f>VLOOKUP(F10,Options!C$2:D$100,2,FALSE)</f>
@@ -851,29 +966,37 @@
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="3" t="str">
-        <f t="shared" ref="I10:I15" si="2">CONCATENATE("#define ",A10," GPIO(",B10,", ",C10,", ",D10,", ",F10,")")</f>
+        <f t="shared" ref="I10:I15" si="4">CONCATENATE("#define ",A10," GPIO(",B10,", ",C10,", ",D10,", ",F10,")")</f>
         <v>#define PX_GPIO_A0 GPIO(C, 0, PX_GPIO_DIR_IN, PX_GPIO_INIT_HIZ)</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K10" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>static const px_gpio_handle_t px_gpio_a0 = {PX_GPIO_A0};</v>
+      </c>
+      <c r="M10" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>#define PX_GPIO_C0 PX_GPIO_A0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" s="4">
         <v>1</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E11" s="6">
         <f>VLOOKUP(D11,Options!A$2:B$100,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G11" s="6">
         <f>VLOOKUP(F11,Options!C$2:D$100,2,FALSE)</f>
@@ -881,29 +1004,37 @@
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>#define PX_GPIO_A1 GPIO(C, 1, PX_GPIO_DIR_IN, PX_GPIO_INIT_HIZ)</v>
+      </c>
+      <c r="K11" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>static const px_gpio_handle_t px_gpio_a1 = {PX_GPIO_A1};</v>
+      </c>
+      <c r="M11" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>#define PX_GPIO_A1 GPIO(C, 1, PX_GPIO_DIR_IN, PX_GPIO_INIT_HIZ)</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+        <v>#define PX_GPIO_C1 PX_GPIO_A1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12" s="4">
         <v>2</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E12" s="6">
         <f>VLOOKUP(D12,Options!A$2:B$100,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G12" s="6">
         <f>VLOOKUP(F12,Options!C$2:D$100,2,FALSE)</f>
@@ -911,29 +1042,37 @@
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>#define PX_GPIO_A2 GPIO(C, 2, PX_GPIO_DIR_IN, PX_GPIO_INIT_HIZ)</v>
+      </c>
+      <c r="K12" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>static const px_gpio_handle_t px_gpio_a2 = {PX_GPIO_A2};</v>
+      </c>
+      <c r="M12" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>#define PX_GPIO_A2 GPIO(C, 2, PX_GPIO_DIR_IN, PX_GPIO_INIT_HIZ)</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <v>#define PX_GPIO_C2 PX_GPIO_A2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13" s="4">
         <v>3</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E13" s="6">
         <f>VLOOKUP(D13,Options!A$2:B$100,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G13" s="6">
         <f>VLOOKUP(F13,Options!C$2:D$100,2,FALSE)</f>
@@ -941,29 +1080,37 @@
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>#define PX_GPIO_A3 GPIO(C, 3, PX_GPIO_DIR_IN, PX_GPIO_INIT_HIZ)</v>
+      </c>
+      <c r="K13" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>static const px_gpio_handle_t px_gpio_a3 = {PX_GPIO_A3};</v>
+      </c>
+      <c r="M13" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>#define PX_GPIO_A3 GPIO(C, 3, PX_GPIO_DIR_IN, PX_GPIO_INIT_HIZ)</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+        <v>#define PX_GPIO_C3 PX_GPIO_A3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" s="4">
         <v>4</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E14" s="6">
         <f>VLOOKUP(D14,Options!A$2:B$100,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G14" s="6">
         <f>VLOOKUP(F14,Options!C$2:D$100,2,FALSE)</f>
@@ -971,29 +1118,37 @@
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>#define PX_GPIO_I2C_SDA GPIO(C, 4, PX_GPIO_DIR_IN, PX_GPIO_INIT_PULLUP)</v>
+      </c>
+      <c r="K14" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>static const px_gpio_handle_t px_gpio_i2c_sda = {PX_GPIO_I2C_SDA};</v>
+      </c>
+      <c r="M14" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>#define PX_GPIO_I2C_SDA GPIO(C, 4, PX_GPIO_DIR_IN, PX_GPIO_INIT_PULLUP)</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+        <v>#define PX_GPIO_C4 PX_GPIO_I2C_SDA</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15" s="4">
         <v>5</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E15" s="6">
         <f>VLOOKUP(D15,Options!A$2:B$100,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G15" s="6">
         <f>VLOOKUP(F15,Options!C$2:D$100,2,FALSE)</f>
@@ -1001,29 +1156,37 @@
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>#define PX_GPIO_I2C_SCL GPIO(C, 5, PX_GPIO_DIR_IN, PX_GPIO_INIT_PULLUP)</v>
+      </c>
+      <c r="K15" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>static const px_gpio_handle_t px_gpio_i2c_scl = {PX_GPIO_I2C_SCL};</v>
+      </c>
+      <c r="M15" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>#define PX_GPIO_I2C_SCL GPIO(C, 5, PX_GPIO_DIR_IN, PX_GPIO_INIT_PULLUP)</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+        <v>#define PX_GPIO_C5 PX_GPIO_I2C_SCL</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C17" s="4">
         <v>0</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E17" s="6">
         <f>VLOOKUP(D17,Options!A$2:B$100,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G17" s="6">
         <f>VLOOKUP(F17,Options!C$2:D$100,2,FALSE)</f>
@@ -1031,29 +1194,37 @@
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="3" t="str">
-        <f t="shared" ref="I17:I24" si="3">CONCATENATE("#define ",A17," GPIO(",B17,", ",C17,", ",D17,", ",F17,")")</f>
+        <f t="shared" ref="I17:I24" si="5">CONCATENATE("#define ",A17," GPIO(",B17,", ",C17,", ",D17,", ",F17,")")</f>
         <v>#define PX_GPIO_UART_RXD GPIO(D, 0, PX_GPIO_DIR_IN, PX_GPIO_INIT_PULLUP)</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K17" s="3" t="str">
+        <f t="shared" ref="K17:K24" si="6">CONCATENATE("static const px_gpio_handle_t ",LOWER($A17)," = {",$A17,"};")</f>
+        <v>static const px_gpio_handle_t px_gpio_uart_rxd = {PX_GPIO_UART_RXD};</v>
+      </c>
+      <c r="M17" s="3" t="str">
+        <f t="shared" ref="M17:M24" si="7">CONCATENATE("#define PX_GPIO_",$B17,$C17," ",$A17)</f>
+        <v>#define PX_GPIO_D0 PX_GPIO_UART_RXD</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" s="4">
         <v>1</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E18" s="6">
         <f>VLOOKUP(D18,Options!A$2:B$100,2,FALSE)</f>
         <v>2</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G18" s="6">
         <f>VLOOKUP(F18,Options!C$2:D$100,2,FALSE)</f>
@@ -1061,29 +1232,37 @@
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#define PX_GPIO_UART_TXD GPIO(D, 1, PX_GPIO_DIR_OUT, PX_GPIO_INIT_HI)</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K18" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>static const px_gpio_handle_t px_gpio_uart_txd = {PX_GPIO_UART_TXD};</v>
+      </c>
+      <c r="M18" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>#define PX_GPIO_D1 PX_GPIO_UART_TXD</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19" s="4">
         <v>2</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E19" s="6">
         <f>VLOOKUP(D19,Options!A$2:B$100,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G19" s="6">
         <f>VLOOKUP(F19,Options!C$2:D$100,2,FALSE)</f>
@@ -1091,29 +1270,37 @@
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#define PX_GPIO_D2 GPIO(D, 2, PX_GPIO_DIR_IN, PX_GPIO_INIT_PULLUP)</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K19" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>static const px_gpio_handle_t px_gpio_d2 = {PX_GPIO_D2};</v>
+      </c>
+      <c r="M19" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>#define PX_GPIO_D2 PX_GPIO_D2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C20" s="4">
         <v>3</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E20" s="6">
         <f>VLOOKUP(D20,Options!A$2:B$100,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G20" s="6">
         <f>VLOOKUP(F20,Options!C$2:D$100,2,FALSE)</f>
@@ -1121,29 +1308,37 @@
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#define PX_GPIO_D3 GPIO(D, 3, PX_GPIO_DIR_IN, PX_GPIO_INIT_PULLUP)</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K20" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>static const px_gpio_handle_t px_gpio_d3 = {PX_GPIO_D3};</v>
+      </c>
+      <c r="M20" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>#define PX_GPIO_D3 PX_GPIO_D3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C21" s="4">
         <v>4</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E21" s="6">
         <f>VLOOKUP(D21,Options!A$2:B$100,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G21" s="6">
         <f>VLOOKUP(F21,Options!C$2:D$100,2,FALSE)</f>
@@ -1151,29 +1346,37 @@
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#define PX_GPIO_D4 GPIO(D, 4, PX_GPIO_DIR_IN, PX_GPIO_INIT_PULLUP)</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K21" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>static const px_gpio_handle_t px_gpio_d4 = {PX_GPIO_D4};</v>
+      </c>
+      <c r="M21" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>#define PX_GPIO_D4 PX_GPIO_D4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" s="4">
         <v>5</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E22" s="6">
         <f>VLOOKUP(D22,Options!A$2:B$100,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G22" s="6">
         <f>VLOOKUP(F22,Options!C$2:D$100,2,FALSE)</f>
@@ -1181,29 +1384,37 @@
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#define PX_GPIO_D5 GPIO(D, 5, PX_GPIO_DIR_IN, PX_GPIO_INIT_PULLUP)</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K22" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>static const px_gpio_handle_t px_gpio_d5 = {PX_GPIO_D5};</v>
+      </c>
+      <c r="M22" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>#define PX_GPIO_D5 PX_GPIO_D5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C23" s="4">
         <v>6</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E23" s="6">
         <f>VLOOKUP(D23,Options!A$2:B$100,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G23" s="6">
         <f>VLOOKUP(F23,Options!C$2:D$100,2,FALSE)</f>
@@ -1211,29 +1422,37 @@
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#define PX_GPIO_D6 GPIO(D, 6, PX_GPIO_DIR_IN, PX_GPIO_INIT_PULLUP)</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K23" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>static const px_gpio_handle_t px_gpio_d6 = {PX_GPIO_D6};</v>
+      </c>
+      <c r="M23" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>#define PX_GPIO_D6 PX_GPIO_D6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C24" s="4">
         <v>7</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E24" s="6">
         <f>VLOOKUP(D24,Options!A$2:B$100,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G24" s="6">
         <f>VLOOKUP(F24,Options!C$2:D$100,2,FALSE)</f>
@@ -1241,8 +1460,16 @@
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>#define PX_GPIO_D7 GPIO(D, 7, PX_GPIO_DIR_IN, PX_GPIO_INIT_PULLUP)</v>
+      </c>
+      <c r="K24" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>static const px_gpio_handle_t px_gpio_d7 = {PX_GPIO_D7};</v>
+      </c>
+      <c r="M24" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>#define PX_GPIO_D7 PX_GPIO_D7</v>
       </c>
     </row>
   </sheetData>
@@ -1751,10 +1978,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D17:D24 D10:D15 D2:D8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D17:D24 D10:D15 D2:D8" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>Dir</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F17:F24 F2:F8 F10:F15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F17:F24 F2:F8 F10:F15" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>Init</formula1>
     </dataValidation>
   </dataValidations>
@@ -1764,7 +1991,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1782,24 +2009,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" s="4">
         <v>1</v>
@@ -1808,13 +2035,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="4">
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="4">
         <v>2</v>
@@ -1823,7 +2050,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C4" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="4">
         <v>3</v>
@@ -1832,7 +2059,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C5" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="4">
         <v>4</v>

</xml_diff>